<commit_message>
Nang cap logic nhap diem
</commit_message>
<xml_diff>
--- a/Nhap_Diem_Thi.xlsx
+++ b/Nhap_Diem_Thi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAI HOC\Code BTL\Student-Management-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FE4AF1-3409-45F1-A69F-959CBD92B374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867D6DE4-7C42-4147-82D1-40D884031A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F275B775-7D48-4C5F-98D3-0D39680AA23C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>B22DCVT007</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>ma_sinh_vien</t>
+  </si>
+  <si>
+    <t>diem_thuc_hanh</t>
   </si>
 </sst>
 </file>
@@ -564,19 +567,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2AF4A40-D606-4976-916F-13FAC0633FA4}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.21875" customWidth="1"/>
     <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -587,10 +593,13 @@
         <v>47</v>
       </c>
       <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -600,14 +609,18 @@
       </c>
       <c r="C2">
         <f ca="1">MROUND(RAND()*(10-5)+5,0.25)</f>
-        <v>7.75</v>
+        <v>9.5</v>
       </c>
       <c r="D2">
         <f ca="1">MROUND(RAND()*(10-5)+5,0.25)</f>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+      <c r="E2">
+        <f ca="1">MROUND(RAND()*(10-5)+5,0.25)</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -616,15 +629,19 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:D47" ca="1" si="1">MROUND(RAND()*(10-5)+5,0.25)</f>
+        <f t="shared" ref="C3:E47" ca="1" si="1">MROUND(RAND()*(10-5)+5,0.25)</f>
         <v>6.75</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.25</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -634,14 +651,18 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5</v>
+        <v>8.75</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.75</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -651,14 +672,18 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.25</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -668,31 +693,39 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>8.75</v>
+        <v>5.25</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.75</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>9.75</v>
+        <v>9.25</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.25</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -702,48 +735,60 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.75</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.25</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
         <v>7.25</v>
       </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C9">
+      <c r="E9">
         <f t="shared" ca="1" si="1"/>
         <v>7.75</v>
       </c>
-      <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -753,14 +798,18 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -770,65 +819,81 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5</v>
+        <v>5.75</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5</v>
+        <v>8.25</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>6.75</v>
+        <v>7.25</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>9.25</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -838,14 +903,18 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
+        <v>7.75</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.75</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -855,82 +924,102 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="1"/>
         <v>6.75</v>
       </c>
-      <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="1"/>
         <v>5.75</v>
       </c>
-      <c r="D18">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="1"/>
         <v>9.5</v>
       </c>
-      <c r="D19">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9.75</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.75</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -940,82 +1029,102 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>5.25</v>
+        <v>6.25</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
         <v>7.75</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.75</v>
+        <v>5.25</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.25</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
+        <v>5.75</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.75</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>5.75</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.75</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1025,82 +1134,102 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>9.25</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.25</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28">
         <f ca="1">RANDBETWEEN(6,10)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.25</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5</v>
+        <v>5.25</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.75</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C31">
         <f ca="1">RANDBETWEEN(8,10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <f ca="1">RANDBETWEEN(6,10)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <f ca="1">RANDBETWEEN(6,10)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1110,116 +1239,144 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="1"/>
+        <v>7.75</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="1"/>
         <v>9.25</v>
       </c>
-      <c r="D33">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
+        <v>7.75</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.25</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.75</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.75</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="C37">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.75</v>
-      </c>
-      <c r="D37">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="1"/>
-        <v>8.25</v>
+        <v>5.75</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.75</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1229,31 +1386,39 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.25</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="C40">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.75</v>
-      </c>
-      <c r="D40">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1263,14 +1428,18 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="1"/>
-        <v>5.25</v>
+        <v>8.25</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.75</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1280,65 +1449,81 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="1"/>
-        <v>7.25</v>
+        <v>7.75</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ca="1" si="1"/>
         <v>8.75</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
-      <c r="D43">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.75</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="1"/>
-        <v>6.25</v>
+        <v>8.25</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ca="1" si="1"/>
         <v>9.5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1348,28 +1533,36 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="1"/>
-        <v>7.75</v>
+        <v>9.25</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="1"/>
-        <v>7.25</v>
+        <v>5.25</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6.25</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>